<commit_message>
add al to excel file
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10User\Desktop\big project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10User\Desktop\coach rony\web 0\session8 deploy api &amp; install free template\api\team api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5CE19CC-10A5-4B01-AFBF-D94ACFE760FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58218A33-B98A-4A8A-B772-3E984D98D0F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="74">
   <si>
     <t>id</t>
   </si>
@@ -224,13 +224,46 @@
   </si>
   <si>
     <t>Tilda</t>
+  </si>
+  <si>
+    <t>alt</t>
+  </si>
+  <si>
+    <t>team1</t>
+  </si>
+  <si>
+    <t>team2</t>
+  </si>
+  <si>
+    <t>team3</t>
+  </si>
+  <si>
+    <t>team4</t>
+  </si>
+  <si>
+    <t>team5</t>
+  </si>
+  <si>
+    <t>team6</t>
+  </si>
+  <si>
+    <t>team7</t>
+  </si>
+  <si>
+    <t>team8</t>
+  </si>
+  <si>
+    <t>team9</t>
+  </si>
+  <si>
+    <t>team10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,6 +283,12 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -595,16 +634,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83075E54-268F-429D-85C1-2CFE9B6973B4}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1796875" customWidth="1"/>
     <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.08984375" bestFit="1" customWidth="1"/>
@@ -614,7 +653,7 @@
     <col min="9" max="9" width="66.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -642,8 +681,11 @@
       <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="4" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -671,8 +713,11 @@
       <c r="I2" s="5" t="s">
         <v>43</v>
       </c>
+      <c r="J2" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -700,8 +745,11 @@
       <c r="I3" s="5" t="s">
         <v>44</v>
       </c>
+      <c r="J3" t="s">
+        <v>65</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -729,8 +777,11 @@
       <c r="I4" s="5" t="s">
         <v>46</v>
       </c>
+      <c r="J4" t="s">
+        <v>66</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -758,8 +809,11 @@
       <c r="I5" s="5" t="s">
         <v>45</v>
       </c>
+      <c r="J5" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -787,8 +841,11 @@
       <c r="I6" s="5" t="s">
         <v>49</v>
       </c>
+      <c r="J6" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -816,8 +873,11 @@
       <c r="I7" s="5" t="s">
         <v>50</v>
       </c>
+      <c r="J7" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -845,8 +905,11 @@
       <c r="I8" s="5" t="s">
         <v>47</v>
       </c>
+      <c r="J8" t="s">
+        <v>70</v>
+      </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -874,8 +937,11 @@
       <c r="I9" s="5" t="s">
         <v>48</v>
       </c>
+      <c r="J9" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -903,8 +969,11 @@
       <c r="I10" s="5" t="s">
         <v>51</v>
       </c>
+      <c r="J10" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -932,8 +1001,12 @@
       <c r="I11" s="5" t="s">
         <v>52</v>
       </c>
+      <c r="J11" t="s">
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" xr:uid="{CC51632D-1791-49F3-9AF2-5F4E8EFD264E}"/>
     <hyperlink ref="H3:H11" r:id="rId2" display="mostafa@outlook.com" xr:uid="{00818198-C5CB-49F5-864E-1C56011A6C0A}"/>

</xml_diff>